<commit_message>
2kr analysis on minion throughput
2 analysis made, for easy and hard game mode
</commit_message>
<xml_diff>
--- a/Analysis/calibration/factors_calibration/bosses/30_repetitions/boss_calibration_response_time.xlsx
+++ b/Analysis/calibration/factors_calibration/bosses/30_repetitions/boss_calibration_response_time.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -220,7 +220,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,10 +258,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -353,7 +349,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -437,6 +433,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -628,11 +625,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="54762726"/>
-        <c:axId val="76567817"/>
+        <c:axId val="33847687"/>
+        <c:axId val="48719581"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54762726"/>
+        <c:axId val="33847687"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,12 +685,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76567817"/>
+        <c:crossAx val="48719581"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76567817"/>
+        <c:axId val="48719581"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,7 +755,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54762726"/>
+        <c:crossAx val="33847687"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -817,9 +814,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>973440</xdr:colOff>
+      <xdr:colOff>973080</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>72000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -827,8 +824,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12054240" y="3280320"/>
-        <a:ext cx="6641280" cy="4114080"/>
+        <a:off x="12065040" y="3280320"/>
+        <a:ext cx="6641640" cy="4113720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -848,11 +845,11 @@
   </sheetPr>
   <dimension ref="B1:U332"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U25" activeCellId="0" sqref="U25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.88"/>
@@ -861,8 +858,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="25.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="44.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="33.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="44.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="33.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1214,8 +1211,8 @@
         <v>56.5803354605128</v>
       </c>
       <c r="N9" s="6" t="n">
-        <f aca="false">AVERAGE(G$3:G$32)</f>
-        <v>105.7</v>
+        <f aca="false">AVERAGE(G$183:G$212)</f>
+        <v>104.5</v>
       </c>
       <c r="P9" s="0" t="n">
         <f aca="false">_xlfn.STDEV.S($H183:$H212)</f>
@@ -1393,16 +1390,16 @@
         <f aca="false">AVERAGE($H303:$H332)</f>
         <v>843.967567245203</v>
       </c>
-      <c r="N13" s="11" t="n">
+      <c r="N13" s="10" t="n">
         <f aca="false">AVERAGE(G$303:G$332)</f>
         <v>42.9666666666667</v>
       </c>
-      <c r="O13" s="12"/>
+      <c r="O13" s="11"/>
       <c r="P13" s="10" t="n">
         <f aca="false">_xlfn.STDEV.S($H303:$H332)</f>
         <v>134.206851291373</v>
       </c>
-      <c r="Q13" s="13" t="n">
+      <c r="Q13" s="12" t="n">
         <f aca="false">CONFIDENCE(0.05,P13,COUNT(D13:D42))</f>
         <v>48.0244224754489</v>
       </c>
@@ -1616,10 +1613,10 @@
       <c r="I21" s="0" t="n">
         <v>1.15593941146467</v>
       </c>
-      <c r="T21" s="14" t="s">
+      <c r="T21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="U21" s="14" t="s">
+      <c r="U21" s="13" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update calibration and 2kr charts
</commit_message>
<xml_diff>
--- a/Analysis/calibration/factors_calibration/bosses/30_repetitions/boss_calibration_response_time.xlsx
+++ b/Analysis/calibration/factors_calibration/bosses/30_repetitions/boss_calibration_response_time.xlsx
@@ -349,7 +349,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -625,11 +625,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="33847687"/>
-        <c:axId val="48719581"/>
+        <c:axId val="31248374"/>
+        <c:axId val="15830935"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="33847687"/>
+        <c:axId val="31248374"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -650,7 +650,7 @@
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Mean Service Time E[ts] [seconds]</a:t>
+                  <a:t>Mean Service Time E[ts] [s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -685,12 +685,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48719581"/>
+        <c:crossAx val="15830935"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48719581"/>
+        <c:axId val="15830935"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -720,7 +720,7 @@
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Mean Response Time E[R]</a:t>
+                  <a:t>Mean Response Time E[R] [s]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -755,7 +755,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33847687"/>
+        <c:crossAx val="31248374"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -808,15 +808,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>934920</xdr:colOff>
+      <xdr:colOff>174960</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>7200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>973080</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>72000</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>17280</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -824,8 +824,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12065040" y="3280320"/>
-        <a:ext cx="6641640" cy="4113720"/>
+        <a:off x="11316600" y="3280320"/>
+        <a:ext cx="8211600" cy="5085000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -845,11 +845,11 @@
   </sheetPr>
   <dimension ref="B1:U332"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R36" activeCellId="0" sqref="R36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.88"/>

</xml_diff>